<commit_message>
function for generating households
</commit_message>
<xml_diff>
--- a/data/gq.xlsx
+++ b/data/gq.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hana/psrc/R/shinyserver/remi-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18184FF-1FD8-FB4D-BEE5-06B90D9C1F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A12A6A9-8224-DA45-9ED4-629F0436B936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7980" yWindow="2840" windowWidth="27640" windowHeight="16940" xr2:uid="{AB35624E-D3BA-2045-BBC7-77061FCD4155}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -289,7 +289,7 @@
     <xf numFmtId="164" fontId="5" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
@@ -634,7 +634,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A9A480-B1C8-F94A-8BA9-9ABD5ADD9233}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>